<commit_message>
Added xView chipper, DOTA results
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\school\e2cnn_experiments\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{486E71F8-8252-4E0A-ABF6-57A02155BDBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758BC506-C399-4399-A9D9-461B9C9CA971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{99A46D3A-88E6-483C-A546-B2DD2430B372}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{484F53C8-DA1C-4908-B869-EDBB5FA70F7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,21 +34,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Epoch</t>
   </si>
   <si>
-    <t>Train Accuracy</t>
+    <t>Non-Equivariant Test Loss</t>
   </si>
   <si>
-    <t>Train Loss</t>
+    <t xml:space="preserve">Non-Equivariant Test Accuracy    </t>
   </si>
   <si>
-    <t>Test Accuracy</t>
+    <t xml:space="preserve">Equivariant Test Accuracy    </t>
   </si>
   <si>
-    <t>Test Loss</t>
+    <t xml:space="preserve">Equivariant Test Loss    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Non-Equivariant Train Accuracy    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Equivariant Train Accuracy    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Non-Equivariant Train Loss    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Equivariant Train Loss    </t>
   </si>
 </sst>
 </file>
@@ -137,12 +149,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Model</a:t>
-            </a:r>
-            <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Accuracy</a:t>
+              <a:t>Equivariant vs Non-Equivariant Model</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -151,8 +159,9 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t>E2CNN (C8) - DOTA</a:t>
+              <a:t>Train/Test Accuracy (DOTA)</a:t>
             </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -192,7 +201,7 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
@@ -200,7 +209,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Train Accuracy</c:v>
+                  <c:v> Non-Equivariant Train Accuracy    </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -208,7 +217,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -219,168 +228,159 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$54</c:f>
+              <c:f>Sheet1!$B$2:$B$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="53"/>
+                <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>55.028735632183903</c:v>
+                  <c:v>42.844827586206897</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>62.361947791164603</c:v>
+                  <c:v>55.722891566264998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>66.655435759209297</c:v>
+                  <c:v>61.522911051212901</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>70.877551020408106</c:v>
+                  <c:v>64.989795918367307</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>73.934977578475298</c:v>
+                  <c:v>68.366965620328799</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>76.155172413793096</c:v>
+                  <c:v>71.043103448275801</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>78.862763915547006</c:v>
+                  <c:v>72.640754958413297</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>80.388059701492494</c:v>
+                  <c:v>74.828358208955194</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>82.256711409395905</c:v>
+                  <c:v>75.908836689037997</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>83.486842105263094</c:v>
+                  <c:v>77.631578947368396</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>85.028564331843</c:v>
+                  <c:v>78.595380029806194</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>86.364705882352894</c:v>
+                  <c:v>79.423529411764704</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>86.243297587131295</c:v>
+                  <c:v>80.9707327971403</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>87.798889837745506</c:v>
+                  <c:v>81.009820666097298</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>88.600532350532305</c:v>
+                  <c:v>82.033169533169499</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>88.985051140833903</c:v>
+                  <c:v>82.980920535011805</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>90.755102040816297</c:v>
+                  <c:v>83.301707779886101</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>90.785714285714207</c:v>
+                  <c:v>84.070877708409796</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>91.520351157222606</c:v>
+                  <c:v>84.915480427046205</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>91.003122560499605</c:v>
+                  <c:v>85.261838921534704</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>91.424751718869302</c:v>
+                  <c:v>86.004885444743906</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>91.6666666666666</c:v>
+                  <c:v>86.210154452842502</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>92.112005856515296</c:v>
+                  <c:v>86.401539448364304</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>91.938665710186498</c:v>
+                  <c:v>87.034137175070398</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>92.528129395218002</c:v>
+                  <c:v>87.672123623011004</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>92.146551724137893</c:v>
+                  <c:v>87.885133113969403</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>92.642083897158301</c:v>
+                  <c:v>88.052223522527797</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>92.936586985391699</c:v>
+                  <c:v>88.280131691955305</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>92.853650586701406</c:v>
+                  <c:v>88.873318385650194</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>93.1381957773512</c:v>
+                  <c:v>89.335712325006796</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>93.156819610307906</c:v>
+                  <c:v>89.248251748251704</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>93.638048177887498</c:v>
+                  <c:v>89.289480622198795</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>93.154219793563996</c:v>
+                  <c:v>90.001292657704198</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>93.514925373134304</c:v>
+                  <c:v>90.537027643925896</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>93.650910158543695</c:v>
+                  <c:v>90.4927824788452</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>94.129116117850899</c:v>
+                  <c:v>90.877718055216206</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>94.073337123365505</c:v>
+                  <c:v>91.404750479846399</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>94.050615212527902</c:v>
+                  <c:v>91.515437190666901</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>93.928964757709196</c:v>
+                  <c:v>91.500694766095407</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>94.116052060737502</c:v>
+                  <c:v>91.728317778283596</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>92.267189758414204</c:v>
+                  <c:v>91.993061772605103</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>92.863345521023703</c:v>
+                  <c:v>92.083975346687197</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>92.950167504187604</c:v>
+                  <c:v>92.393893460372396</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>93.052118775131405</c:v>
+                  <c:v>92.275729810355799</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>93.361716123373697</c:v>
+                  <c:v>92.745910234899299</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>93.640867516629697</c:v>
+                  <c:v>92.631117076192396</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>94.075220656040003</c:v>
+                  <c:v>92.961906701975906</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>94.195643986944503</c:v>
+                  <c:v>93.229585679806902</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>94.601966191104097</c:v>
+                  <c:v>93.129221295192593</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>94.895881138136701</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>95.246672533274605</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>95.544580604267907</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>95.631290027447307</c:v>
+                  <c:v>93.309790072591696</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -388,12 +388,12 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-B6E9-4B3F-9EF0-8B23BC1FF10E}"/>
+              <c16:uniqueId val="{00000001-2DFF-4493-99BE-9A426B86CF60}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="3"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
@@ -401,7 +401,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Test Accuracy</c:v>
+                  <c:v>Non-Equivariant Test Accuracy    </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -409,7 +409,200 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>50.548002219755801</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>61.757769145394001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60.3218645948945</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64.421476137624794</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>67.463235294117595</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>67.081714761376205</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>73.2241953385127</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>75.548002219755801</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>73.293562708102101</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>76.338790233074306</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>76.422031076581504</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>77.018590455049903</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>76.931881243063202</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>77.139983351831305</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>78.003607103218599</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>79.796753607103199</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>78.648723640399496</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>80.323945615982197</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>79.481132075471606</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>80.261514983351802</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>81.038429522752494</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>82.422308546059895</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>82.158712541620403</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>80.774833518312903</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>82.592258601553795</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>82.977247502774702</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>83.199223085460503</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>81.634988901220794</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>82.151775804661398</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>83.820061043285193</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>83.084766925638107</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>82.682436182019899</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>83.764567147613704</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>84.267480577136496</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>83.833934517203105</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>83.525249722530504</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>84.978496115427305</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>83.743756936736901</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>83.039678135405097</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>85.092952275249701</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>84.721836847946705</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>84.995837957824605</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>84.610849056603698</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>84.621254162042106</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>85.242092119866797</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>84.985432852386197</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>85.464067702552697</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>85.200471698113205</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>85.658296337402803</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>85.491814650388406</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-2DFF-4493-99BE-9A426B86CF60}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> Equivariant Train Accuracy    </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -420,168 +613,159 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$54</c:f>
+              <c:f>Sheet1!$F$2:$F$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="53"/>
+                <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>60.980854605993301</c:v>
+                  <c:v>41.264367816091898</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>68.746531631520497</c:v>
+                  <c:v>56.739457831325304</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>68.486403995560394</c:v>
+                  <c:v>64.555256064689999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>72.551331853496094</c:v>
+                  <c:v>69.030612244897895</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>70.910793562708093</c:v>
+                  <c:v>72.281390134529104</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>73.740982241953304</c:v>
+                  <c:v>75.568965517241296</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>74.243895671476096</c:v>
+                  <c:v>77.815099168266102</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>76.154966703662595</c:v>
+                  <c:v>80.104477611940297</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>74.923695893451693</c:v>
+                  <c:v>81.403803131990998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>76.824361820199698</c:v>
+                  <c:v>83.506578947368396</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>76.338790233074306</c:v>
+                  <c:v>84.401390958768005</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>75.957269700332901</c:v>
+                  <c:v>85.417647058823505</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>78.385127635960004</c:v>
+                  <c:v>86.868856121536993</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>78.718091009988896</c:v>
+                  <c:v>87.980358667805206</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>78.9782186459489</c:v>
+                  <c:v>88.380425880425804</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>81.0106825749167</c:v>
+                  <c:v>88.940794649881894</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>77.871809100998803</c:v>
+                  <c:v>89.454459203035995</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>80.1054384017758</c:v>
+                  <c:v>90.231362467866305</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>80.490427302996594</c:v>
+                  <c:v>90.275800711743699</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>79.821032186459405</c:v>
+                  <c:v>91.043034911856196</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>80.008324084350704</c:v>
+                  <c:v>91.084063342318004</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>79.8661209766925</c:v>
+                  <c:v>92.076076240551998</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>80.826859045504904</c:v>
+                  <c:v>91.861770365618995</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>81.586431742508296</c:v>
+                  <c:v>92.405261509552105</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>80.982935627081005</c:v>
+                  <c:v>92.480110159118695</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>80.674250832408404</c:v>
+                  <c:v>92.850732874663393</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>81.725166481686998</c:v>
+                  <c:v>93.099034523112906</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>82.196864594894507</c:v>
+                  <c:v>93.3116232464929</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>81.159822419533796</c:v>
+                  <c:v>93.497757847533606</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>80.573668146503806</c:v>
+                  <c:v>93.816909140817998</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>80.306603773584897</c:v>
+                  <c:v>93.884480903711605</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>79.658018867924497</c:v>
+                  <c:v>93.952675982072194</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>81.083518312985504</c:v>
+                  <c:v>94.040847983453901</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>80.452275249722504</c:v>
+                  <c:v>94.4521937610956</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>81.170227524972205</c:v>
+                  <c:v>94.577526132404103</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>81.409544950055405</c:v>
+                  <c:v>94.612753481553796</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>81.891648168701394</c:v>
+                  <c:v>94.964611324376193</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>80.663845726969996</c:v>
+                  <c:v>95.268677822295501</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>81.319367369589301</c:v>
+                  <c:v>95.093214451134699</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>82.630410654827898</c:v>
+                  <c:v>95.398930116093695</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>81.506659267480501</c:v>
+                  <c:v>95.551700984780595</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>82.571448390677006</c:v>
+                  <c:v>95.578362315650395</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>83.109045504994398</c:v>
+                  <c:v>95.839649198787299</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>82.450055493895604</c:v>
+                  <c:v>95.759642020029801</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>83.719478357380595</c:v>
+                  <c:v>95.949559563758299</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>84.270948945615899</c:v>
+                  <c:v>96.012285773280993</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>83.660516093229703</c:v>
+                  <c:v>96.223772662456696</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>83.684794672585994</c:v>
+                  <c:v>96.108205953338697</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>83.854744728079893</c:v>
+                  <c:v>96.208283671036895</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>83.605022197558199</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>83.9483906770255</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>84.048973362929999</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>84.080188679245197</c:v>
+                  <c:v>96.363056700019598</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -589,7 +773,200 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-B6E9-4B3F-9EF0-8B23BC1FF10E}"/>
+              <c16:uniqueId val="{00000005-2DFF-4493-99BE-9A426B86CF60}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Equivariant Test Accuracy    </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$2:$H$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>58.358768035516</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>61.792452830188601</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>69.537319644839002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>72.159406215316295</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>71.229883462819004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>71.649556048834597</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>74.1294395116537</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>77.750416204217501</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>76.869450610432807</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>77.896087680355095</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>76.515677025527197</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>78.284544950055405</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>80.091564927857902</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>79.092674805771296</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>77.750416204217501</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>78.562014428412795</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>79.897336293007697</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>80.906631520532699</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>80.025665926748005</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>81.312430632630395</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>80.934378468368394</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>80.476553829078796</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>81.902053274139803</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>80.795643729189706</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>81.527469478357304</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>81.610710321864602</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>82.037319644839002</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>81.749445061043204</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>81.707824639289598</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>82.6165371809101</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>82.977247502774702</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>82.373751387347397</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>82.959905660377302</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>83.216564927857902</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>83.157602663706996</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>83.480160932297395</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>82.1552441731409</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>83.809655937846799</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>83.240843507214194</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>82.491675915649196</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>82.561043285238597</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>83.396920088790196</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>83.2824639289678</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>83.220033296337405</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>83.376109877913393</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>83.820061043285193</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>83.188817980022193</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>83.792314095449498</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>83.4350721420643</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>82.921753607103199</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-2DFF-4493-99BE-9A426B86CF60}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -602,11 +979,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1759801744"/>
-        <c:axId val="1759802160"/>
+        <c:axId val="705170864"/>
+        <c:axId val="705184176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1759801744"/>
+        <c:axId val="705170864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -703,7 +1080,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1759802160"/>
+        <c:crossAx val="705184176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -711,11 +1088,11 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1759802160"/>
+        <c:axId val="705184176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
-          <c:min val="50"/>
+          <c:min val="40"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -819,10 +1196,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1759801744"/>
+        <c:crossAx val="705170864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="10"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -834,6 +1210,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10597003499562553"/>
+          <c:y val="0.80902668416447965"/>
+          <c:w val="0.87972659667541553"/>
+          <c:h val="0.14930664916885386"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -941,12 +1327,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Model</a:t>
-            </a:r>
-            <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Loss</a:t>
+              <a:t>Equivariant vs Non-Equivariant Model</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -955,8 +1337,9 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t>E2CNN (C8) - DOTA</a:t>
+              <a:t>Train/Test Loss (DOTA)</a:t>
             </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -996,7 +1379,7 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
@@ -1004,7 +1387,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Train Loss</c:v>
+                  <c:v> Non-Equivariant Train Loss    </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1012,7 +1395,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1023,168 +1406,159 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$54</c:f>
+              <c:f>Sheet1!$C$2:$C$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="53"/>
+                <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>1310.97375488281</c:v>
+                  <c:v>1607.33154296875</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1285.11938476562</c:v>
+                  <c:v>1490.30236816406</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1278.37683105468</c:v>
+                  <c:v>1452.58337402343</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1216.30590820312</c:v>
+                  <c:v>1436.11560058593</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1211.5849609375</c:v>
+                  <c:v>1441.68371582031</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1200.04223632812</c:v>
+                  <c:v>1410.92224121093</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1145.1376953125</c:v>
+                  <c:v>1425.19616699218</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1138.021484375</c:v>
+                  <c:v>1409.80615234375</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1085.25134277343</c:v>
+                  <c:v>1441.05676269531</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1082.2802734375</c:v>
+                  <c:v>1407.78637695312</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1041.82751464843</c:v>
+                  <c:v>1413.96813964843</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1006.44006347656</c:v>
+                  <c:v>1437.17456054687</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1013.5728149414</c:v>
+                  <c:v>1407.61218261718</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>974.484619140625</c:v>
+                  <c:v>1435.78881835937</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>944.64141845703102</c:v>
+                  <c:v>1419.01525878906</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>938.18835449218705</c:v>
+                  <c:v>1394.48937988281</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>390.15744018554602</c:v>
+                  <c:v>1410.00244140625</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>383.10336303710898</c:v>
+                  <c:v>1407.08227539062</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>372.74148559570301</c:v>
+                  <c:v>1352.05944824218</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>388.44104003906199</c:v>
+                  <c:v>1356.9970703125</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>378.25518798828102</c:v>
+                  <c:v>1325.97546386718</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>365.688385009765</c:v>
+                  <c:v>1313.13891601562</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>365.0380859375</c:v>
+                  <c:v>1336.701171875</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>375.25775146484301</c:v>
+                  <c:v>1300.89575195312</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>357.82943725585898</c:v>
+                  <c:v>1262.611328125</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>369.75750732421801</c:v>
+                  <c:v>1286.38903808593</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>361.91903686523398</c:v>
+                  <c:v>1269.45593261718</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>345.54544067382801</c:v>
+                  <c:v>1268.26306152343</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>364.434967041015</c:v>
+                  <c:v>1246.509765625</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>342.32687377929602</c:v>
+                  <c:v>1225.48474121093</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>350.34808349609301</c:v>
+                  <c:v>1244.13098144531</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>336.04794311523398</c:v>
+                  <c:v>1240.15295410156</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>366.02056884765602</c:v>
+                  <c:v>1186.21240234375</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>355.20574951171801</c:v>
+                  <c:v>1171.10534667968</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>342.49667358398398</c:v>
+                  <c:v>1170.17785644531</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>338.94680786132801</c:v>
+                  <c:v>1155.0625</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>349.64431762695301</c:v>
+                  <c:v>1106.51745605468</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>351.19265747070301</c:v>
+                  <c:v>1104.1455078125</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>349.62228393554602</c:v>
+                  <c:v>1120.23229980468</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>354.74203491210898</c:v>
+                  <c:v>1117.91198730468</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1178.91967773437</c:v>
+                  <c:v>1110.51672363281</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1242.81567382812</c:v>
+                  <c:v>1086.02966308593</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1300.27978515625</c:v>
+                  <c:v>1073.27416992187</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1369.96936035156</c:v>
+                  <c:v>1085.75952148437</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1382.3056640625</c:v>
+                  <c:v>1053.72888183593</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1365.76428222656</c:v>
+                  <c:v>1065.38354492187</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1352.654296875</c:v>
+                  <c:v>1045.51782226562</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1383.27502441406</c:v>
+                  <c:v>1012.60174560546</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1338.25512695312</c:v>
+                  <c:v>1024.84387207031</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1315.97595214843</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>1304.38024902343</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>1270.52404785156</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>1259.90454101562</c:v>
+                  <c:v>1012.53485107421</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1192,12 +1566,12 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3D1F-40BD-85EC-18406FBEC723}"/>
+              <c16:uniqueId val="{00000000-CFE3-4F7E-9F5F-AE66684FAFDE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="3"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
@@ -1205,7 +1579,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Test Loss</c:v>
+                  <c:v>Non-Equivariant Test Loss</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1213,7 +1587,200 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>5837.7333984375</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4529.2431640625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4652.4130859375</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4196.1328125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3829.69067382812</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3855.5078125</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3140.12719726562</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2879.90698242187</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3133.69287109375</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2827.35571289062</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2753.36254882812</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2680.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2645.00219726562</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2601.80517578125</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2576.7421875</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2351.2900390625</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2430.77172851562</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2365.47314453125</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2387.31640625</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2215.7861328125</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2175.44970703125</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2079.06616210937</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2091.509765625</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2254.86450195312</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2017.42016601562</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2004.97253417968</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1905.11328125</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2140.55859375</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2078.16845703125</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1905.72534179687</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1978.43786621093</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2013.41235351562</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1897.64978027343</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1813.25109863281</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1879.61987304687</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1940.25573730468</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1771.0947265625</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1905.68225097656</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1982.71911621093</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1796.28869628906</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1827.52429199218</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1824.94543457031</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1827.40759277343</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1886.86938476562</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1792.50744628906</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1849.029296875</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1786.01525878906</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1798.9091796875</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1762.57202148437</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1774.80822753906</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-CFE3-4F7E-9F5F-AE66684FAFDE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> Equivariant Train Loss    </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1224,168 +1791,159 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$54</c:f>
+              <c:f>Sheet1!$G$2:$G$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="53"/>
+                <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>4779.16845703125</c:v>
+                  <c:v>1630.26550292968</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3909.74731445312</c:v>
+                  <c:v>1454.18530273437</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3884.19604492187</c:v>
+                  <c:v>1383.26770019531</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3421.125</c:v>
+                  <c:v>1329.5546875</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3462.22827148437</c:v>
+                  <c:v>1286.12463378906</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3091.59814453125</c:v>
+                  <c:v>1246.18518066406</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3047.26147460937</c:v>
+                  <c:v>1198.25012207031</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2815.08178710937</c:v>
+                  <c:v>1152.22106933593</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2886.4580078125</c:v>
+                  <c:v>1157.79541015625</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2775.4990234375</c:v>
+                  <c:v>1088.81018066406</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2819.52978515625</c:v>
+                  <c:v>1073.6552734375</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2850.267578125</c:v>
+                  <c:v>1044.4521484375</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2452.07568359375</c:v>
+                  <c:v>1010.49407958984</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2491.67211914062</c:v>
+                  <c:v>965.23443603515602</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2493.9736328125</c:v>
+                  <c:v>956.15319824218705</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2261.88623046875</c:v>
+                  <c:v>921.245849609375</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2643.53930664062</c:v>
+                  <c:v>925.59344482421795</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2333.45727539062</c:v>
+                  <c:v>907.12017822265602</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2307.4990234375</c:v>
+                  <c:v>885.81170654296795</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2361.34643554687</c:v>
+                  <c:v>865.63342285156205</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2422.71215820312</c:v>
+                  <c:v>852.847412109375</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2390.15991210937</c:v>
+                  <c:v>794.68450927734295</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2301.91918945312</c:v>
+                  <c:v>820.796630859375</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2194.69458007812</c:v>
+                  <c:v>781.921875</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2292.12841796875</c:v>
+                  <c:v>783.07574462890602</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2288.2412109375</c:v>
+                  <c:v>770.153076171875</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2233.74194335937</c:v>
+                  <c:v>755.082763671875</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2151.04418945312</c:v>
+                  <c:v>751.94622802734295</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2282.61254882812</c:v>
+                  <c:v>746.01080322265602</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2352.2705078125</c:v>
+                  <c:v>717.19439697265602</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2466.52880859375</c:v>
+                  <c:v>715.03570556640602</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2523.54565429687</c:v>
+                  <c:v>714.18878173828102</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2379.1025390625</c:v>
+                  <c:v>711.91174316406205</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2477.80151367187</c:v>
+                  <c:v>672.05303955078102</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2334.94311523437</c:v>
+                  <c:v>677.02142333984295</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2334.84643554687</c:v>
+                  <c:v>664.48504638671795</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2239.37817382812</c:v>
+                  <c:v>644.64056396484295</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2431.49682617187</c:v>
+                  <c:v>629.73883056640602</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2337.61962890625</c:v>
+                  <c:v>653.90740966796795</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2258.861328125</c:v>
+                  <c:v>626.82470703125</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2292.0498046875</c:v>
+                  <c:v>614.77990722656205</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>2180.37182617187</c:v>
+                  <c:v>620.25762939453102</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>2101.32934570312</c:v>
+                  <c:v>587.20587158203102</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>2157.23950195312</c:v>
+                  <c:v>606.40142822265602</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2072.63012695312</c:v>
+                  <c:v>589.73431396484295</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>2024.6484375</c:v>
+                  <c:v>584.05822753906205</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>2116.25537109375</c:v>
+                  <c:v>573.69512939453102</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>2113.1572265625</c:v>
+                  <c:v>574.67864990234295</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>2127.11254882812</c:v>
+                  <c:v>572.38702392578102</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>2225.474609375</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>2207.3984375</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>2180.703125</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>2233.845703125</c:v>
+                  <c:v>559.172119140625</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1393,7 +1951,200 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-3D1F-40BD-85EC-18406FBEC723}"/>
+              <c16:uniqueId val="{00000002-CFE3-4F7E-9F5F-AE66684FAFDE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Equivariant Test Loss    </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$2:$I$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>5214.62060546875</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4491.5380859375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3718.48193359375</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3432.36743164062</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3483.38500976562</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3453.9736328125</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3074.79296875</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2706.31298828125</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2694.23828125</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2539.29907226562</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2675.58764648437</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2557.373046875</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2329.53051757812</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2448.77465820312</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2605.43139648437</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2552.91088867187</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2413.49291992187</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2277.29858398437</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2331.18579101562</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2191.30834960937</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2291.72509765625</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2327.4306640625</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2123.58569335937</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2332.88623046875</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2239.87548828125</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2245.26635742187</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2217.97143554687</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2305.20751953125</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2293.68505859375</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2216.39794921875</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2135.60034179687</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2218.849609375</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2144.63012695312</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2113.85815429687</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2204.31298828125</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2164.56689453125</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2353.33618164062</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2162.04711914062</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2204.69799804687</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2293.16943359375</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2363.4287109375</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2288.3818359375</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2253.14233398437</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2256.29711914062</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2288.77709960937</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2209.47607421875</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2347.05859375</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2233.3525390625</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2343.8125</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2359.9111328125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-CFE3-4F7E-9F5F-AE66684FAFDE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1406,11 +2157,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1759801744"/>
-        <c:axId val="1759802160"/>
+        <c:axId val="705170864"/>
+        <c:axId val="705184176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1759801744"/>
+        <c:axId val="705170864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1507,7 +2258,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1759802160"/>
+        <c:crossAx val="705184176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1515,10 +2266,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1759802160"/>
+        <c:axId val="705184176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="5000"/>
+          <c:max val="6000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1622,7 +2373,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1759801744"/>
+        <c:crossAx val="705170864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1636,6 +2387,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.18738692038495186"/>
+          <c:y val="0.79976742490522013"/>
+          <c:w val="0.78633727034120726"/>
+          <c:h val="0.16782516768737238"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2825,23 +3586,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>147637</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>452437</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{685C882F-8D87-40F5-B97C-D2461DAFCF7D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D9C4B3E-D70F-46FC-90BB-A6BC16900214}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2861,23 +3622,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB4266D1-B4D1-4B3A-8D39-5146CA401A5A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2685CCF8-9B05-45EB-9165-7810CBBE46DC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3196,946 +3957,1790 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{527097A4-5DD1-44E6-BC30-4FF732B98428}">
-  <dimension ref="A1:K54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B4BF5B5-05A3-48CF-A4D4-072BBB026293}">
+  <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>55.028735632183903</v>
+        <v>42.844827586206897</v>
       </c>
       <c r="C2">
-        <v>1310.97375488281</v>
+        <v>1607.33154296875</v>
       </c>
       <c r="D2">
-        <v>60.980854605993301</v>
+        <v>50.548002219755801</v>
       </c>
       <c r="E2">
-        <v>4779.16845703125</v>
+        <v>5837.7333984375</v>
+      </c>
+      <c r="F2">
+        <v>41.264367816091898</v>
       </c>
       <c r="G2">
-        <v>-1</v>
+        <v>1630.26550292968</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>58.358768035516</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>3.0382907880133101</v>
-      </c>
-      <c r="K2">
-        <v>503410.03125</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <v>5214.62060546875</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>62.361947791164603</v>
+        <v>55.722891566264998</v>
       </c>
       <c r="C3">
-        <v>1285.11938476562</v>
+        <v>1490.30236816406</v>
       </c>
       <c r="D3">
-        <v>68.746531631520497</v>
+        <v>61.757769145394001</v>
       </c>
       <c r="E3">
-        <v>3909.74731445312</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>4529.2431640625</v>
+      </c>
+      <c r="F3">
+        <v>56.739457831325304</v>
+      </c>
+      <c r="G3">
+        <v>1454.18530273437</v>
+      </c>
+      <c r="H3">
+        <v>61.792452830188601</v>
+      </c>
+      <c r="I3">
+        <v>4491.5380859375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>66.655435759209297</v>
+        <v>61.522911051212901</v>
       </c>
       <c r="C4">
-        <v>1278.37683105468</v>
+        <v>1452.58337402343</v>
       </c>
       <c r="D4">
-        <v>68.486403995560394</v>
+        <v>60.3218645948945</v>
       </c>
       <c r="E4">
-        <v>3884.19604492187</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>4652.4130859375</v>
+      </c>
+      <c r="F4">
+        <v>64.555256064689999</v>
+      </c>
+      <c r="G4">
+        <v>1383.26770019531</v>
+      </c>
+      <c r="H4">
+        <v>69.537319644839002</v>
+      </c>
+      <c r="I4">
+        <v>3718.48193359375</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>70.877551020408106</v>
+        <v>64.989795918367307</v>
       </c>
       <c r="C5">
-        <v>1216.30590820312</v>
+        <v>1436.11560058593</v>
       </c>
       <c r="D5">
-        <v>72.551331853496094</v>
+        <v>64.421476137624794</v>
       </c>
       <c r="E5">
-        <v>3421.125</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>4196.1328125</v>
+      </c>
+      <c r="F5">
+        <v>69.030612244897895</v>
+      </c>
+      <c r="G5">
+        <v>1329.5546875</v>
+      </c>
+      <c r="H5">
+        <v>72.159406215316295</v>
+      </c>
+      <c r="I5">
+        <v>3432.36743164062</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>73.934977578475298</v>
+        <v>68.366965620328799</v>
       </c>
       <c r="C6">
-        <v>1211.5849609375</v>
+        <v>1441.68371582031</v>
       </c>
       <c r="D6">
-        <v>70.910793562708093</v>
+        <v>67.463235294117595</v>
       </c>
       <c r="E6">
-        <v>3462.22827148437</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3829.69067382812</v>
+      </c>
+      <c r="F6">
+        <v>72.281390134529104</v>
+      </c>
+      <c r="G6">
+        <v>1286.12463378906</v>
+      </c>
+      <c r="H6">
+        <v>71.229883462819004</v>
+      </c>
+      <c r="I6">
+        <v>3483.38500976562</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>76.155172413793096</v>
+        <v>71.043103448275801</v>
       </c>
       <c r="C7">
-        <v>1200.04223632812</v>
+        <v>1410.92224121093</v>
       </c>
       <c r="D7">
-        <v>73.740982241953304</v>
+        <v>67.081714761376205</v>
       </c>
       <c r="E7">
-        <v>3091.59814453125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3855.5078125</v>
+      </c>
+      <c r="F7">
+        <v>75.568965517241296</v>
+      </c>
+      <c r="G7">
+        <v>1246.18518066406</v>
+      </c>
+      <c r="H7">
+        <v>71.649556048834597</v>
+      </c>
+      <c r="I7">
+        <v>3453.9736328125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>78.862763915547006</v>
+        <v>72.640754958413297</v>
       </c>
       <c r="C8">
-        <v>1145.1376953125</v>
+        <v>1425.19616699218</v>
       </c>
       <c r="D8">
-        <v>74.243895671476096</v>
+        <v>73.2241953385127</v>
       </c>
       <c r="E8">
-        <v>3047.26147460937</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3140.12719726562</v>
+      </c>
+      <c r="F8">
+        <v>77.815099168266102</v>
+      </c>
+      <c r="G8">
+        <v>1198.25012207031</v>
+      </c>
+      <c r="H8">
+        <v>74.1294395116537</v>
+      </c>
+      <c r="I8">
+        <v>3074.79296875</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>80.388059701492494</v>
+        <v>74.828358208955194</v>
       </c>
       <c r="C9">
-        <v>1138.021484375</v>
+        <v>1409.80615234375</v>
       </c>
       <c r="D9">
-        <v>76.154966703662595</v>
+        <v>75.548002219755801</v>
       </c>
       <c r="E9">
-        <v>2815.08178710937</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2879.90698242187</v>
+      </c>
+      <c r="F9">
+        <v>80.104477611940297</v>
+      </c>
+      <c r="G9">
+        <v>1152.22106933593</v>
+      </c>
+      <c r="H9">
+        <v>77.750416204217501</v>
+      </c>
+      <c r="I9">
+        <v>2706.31298828125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>82.256711409395905</v>
+        <v>75.908836689037997</v>
       </c>
       <c r="C10">
-        <v>1085.25134277343</v>
+        <v>1441.05676269531</v>
       </c>
       <c r="D10">
-        <v>74.923695893451693</v>
+        <v>73.293562708102101</v>
       </c>
       <c r="E10">
-        <v>2886.4580078125</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+        <v>3133.69287109375</v>
+      </c>
+      <c r="F10">
+        <v>81.403803131990998</v>
+      </c>
+      <c r="G10">
+        <v>1157.79541015625</v>
+      </c>
+      <c r="H10">
+        <v>76.869450610432807</v>
+      </c>
+      <c r="I10">
+        <v>2694.23828125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>83.486842105263094</v>
+        <v>77.631578947368396</v>
       </c>
       <c r="C11">
-        <v>1082.2802734375</v>
+        <v>1407.78637695312</v>
       </c>
       <c r="D11">
-        <v>76.824361820199698</v>
+        <v>76.338790233074306</v>
       </c>
       <c r="E11">
-        <v>2775.4990234375</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2827.35571289062</v>
+      </c>
+      <c r="F11">
+        <v>83.506578947368396</v>
+      </c>
+      <c r="G11">
+        <v>1088.81018066406</v>
+      </c>
+      <c r="H11">
+        <v>77.896087680355095</v>
+      </c>
+      <c r="I11">
+        <v>2539.29907226562</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>85.028564331843</v>
+        <v>78.595380029806194</v>
       </c>
       <c r="C12">
-        <v>1041.82751464843</v>
+        <v>1413.96813964843</v>
       </c>
       <c r="D12">
-        <v>76.338790233074306</v>
+        <v>76.422031076581504</v>
       </c>
       <c r="E12">
-        <v>2819.52978515625</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2753.36254882812</v>
+      </c>
+      <c r="F12">
+        <v>84.401390958768005</v>
+      </c>
+      <c r="G12">
+        <v>1073.6552734375</v>
+      </c>
+      <c r="H12">
+        <v>76.515677025527197</v>
+      </c>
+      <c r="I12">
+        <v>2675.58764648437</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>86.364705882352894</v>
+        <v>79.423529411764704</v>
       </c>
       <c r="C13">
-        <v>1006.44006347656</v>
+        <v>1437.17456054687</v>
       </c>
       <c r="D13">
-        <v>75.957269700332901</v>
+        <v>77.018590455049903</v>
       </c>
       <c r="E13">
-        <v>2850.267578125</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2680.5</v>
+      </c>
+      <c r="F13">
+        <v>85.417647058823505</v>
+      </c>
+      <c r="G13">
+        <v>1044.4521484375</v>
+      </c>
+      <c r="H13">
+        <v>78.284544950055405</v>
+      </c>
+      <c r="I13">
+        <v>2557.373046875</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>86.243297587131295</v>
+        <v>80.9707327971403</v>
       </c>
       <c r="C14">
-        <v>1013.5728149414</v>
+        <v>1407.61218261718</v>
       </c>
       <c r="D14">
-        <v>78.385127635960004</v>
+        <v>76.931881243063202</v>
       </c>
       <c r="E14">
-        <v>2452.07568359375</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2645.00219726562</v>
+      </c>
+      <c r="F14">
+        <v>86.868856121536993</v>
+      </c>
+      <c r="G14">
+        <v>1010.49407958984</v>
+      </c>
+      <c r="H14">
+        <v>80.091564927857902</v>
+      </c>
+      <c r="I14">
+        <v>2329.53051757812</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>87.798889837745506</v>
+        <v>81.009820666097298</v>
       </c>
       <c r="C15">
-        <v>974.484619140625</v>
+        <v>1435.78881835937</v>
       </c>
       <c r="D15">
-        <v>78.718091009988896</v>
+        <v>77.139983351831305</v>
       </c>
       <c r="E15">
-        <v>2491.67211914062</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2601.80517578125</v>
+      </c>
+      <c r="F15">
+        <v>87.980358667805206</v>
+      </c>
+      <c r="G15">
+        <v>965.23443603515602</v>
+      </c>
+      <c r="H15">
+        <v>79.092674805771296</v>
+      </c>
+      <c r="I15">
+        <v>2448.77465820312</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16">
-        <v>88.600532350532305</v>
+        <v>82.033169533169499</v>
       </c>
       <c r="C16">
-        <v>944.64141845703102</v>
+        <v>1419.01525878906</v>
       </c>
       <c r="D16">
-        <v>78.9782186459489</v>
+        <v>78.003607103218599</v>
       </c>
       <c r="E16">
-        <v>2493.9736328125</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2576.7421875</v>
+      </c>
+      <c r="F16">
+        <v>88.380425880425804</v>
+      </c>
+      <c r="G16">
+        <v>956.15319824218705</v>
+      </c>
+      <c r="H16">
+        <v>77.750416204217501</v>
+      </c>
+      <c r="I16">
+        <v>2605.43139648437</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>88.985051140833903</v>
+        <v>82.980920535011805</v>
       </c>
       <c r="C17">
-        <v>938.18835449218705</v>
+        <v>1394.48937988281</v>
       </c>
       <c r="D17">
-        <v>81.0106825749167</v>
+        <v>79.796753607103199</v>
       </c>
       <c r="E17">
-        <v>2261.88623046875</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2351.2900390625</v>
+      </c>
+      <c r="F17">
+        <v>88.940794649881894</v>
+      </c>
+      <c r="G17">
+        <v>921.245849609375</v>
+      </c>
+      <c r="H17">
+        <v>78.562014428412795</v>
+      </c>
+      <c r="I17">
+        <v>2552.91088867187</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>90.755102040816297</v>
+        <v>83.301707779886101</v>
       </c>
       <c r="C18">
-        <v>390.15744018554602</v>
+        <v>1410.00244140625</v>
       </c>
       <c r="D18">
-        <v>77.871809100998803</v>
+        <v>78.648723640399496</v>
       </c>
       <c r="E18">
-        <v>2643.53930664062</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2430.77172851562</v>
+      </c>
+      <c r="F18">
+        <v>89.454459203035995</v>
+      </c>
+      <c r="G18">
+        <v>925.59344482421795</v>
+      </c>
+      <c r="H18">
+        <v>79.897336293007697</v>
+      </c>
+      <c r="I18">
+        <v>2413.49291992187</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>90.785714285714207</v>
+        <v>84.070877708409796</v>
       </c>
       <c r="C19">
-        <v>383.10336303710898</v>
+        <v>1407.08227539062</v>
       </c>
       <c r="D19">
-        <v>80.1054384017758</v>
+        <v>80.323945615982197</v>
       </c>
       <c r="E19">
-        <v>2333.45727539062</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2365.47314453125</v>
+      </c>
+      <c r="F19">
+        <v>90.231362467866305</v>
+      </c>
+      <c r="G19">
+        <v>907.12017822265602</v>
+      </c>
+      <c r="H19">
+        <v>80.906631520532699</v>
+      </c>
+      <c r="I19">
+        <v>2277.29858398437</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20">
-        <v>91.520351157222606</v>
+        <v>84.915480427046205</v>
       </c>
       <c r="C20">
-        <v>372.74148559570301</v>
+        <v>1352.05944824218</v>
       </c>
       <c r="D20">
-        <v>80.490427302996594</v>
+        <v>79.481132075471606</v>
       </c>
       <c r="E20">
-        <v>2307.4990234375</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2387.31640625</v>
+      </c>
+      <c r="F20">
+        <v>90.275800711743699</v>
+      </c>
+      <c r="G20">
+        <v>885.81170654296795</v>
+      </c>
+      <c r="H20">
+        <v>80.025665926748005</v>
+      </c>
+      <c r="I20">
+        <v>2331.18579101562</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>91.003122560499605</v>
+        <v>85.261838921534704</v>
       </c>
       <c r="C21">
-        <v>388.44104003906199</v>
+        <v>1356.9970703125</v>
       </c>
       <c r="D21">
-        <v>79.821032186459405</v>
+        <v>80.261514983351802</v>
       </c>
       <c r="E21">
-        <v>2361.34643554687</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2215.7861328125</v>
+      </c>
+      <c r="F21">
+        <v>91.043034911856196</v>
+      </c>
+      <c r="G21">
+        <v>865.63342285156205</v>
+      </c>
+      <c r="H21">
+        <v>81.312430632630395</v>
+      </c>
+      <c r="I21">
+        <v>2191.30834960937</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22">
-        <v>91.424751718869302</v>
+        <v>86.004885444743906</v>
       </c>
       <c r="C22">
-        <v>378.25518798828102</v>
+        <v>1325.97546386718</v>
       </c>
       <c r="D22">
-        <v>80.008324084350704</v>
+        <v>81.038429522752494</v>
       </c>
       <c r="E22">
-        <v>2422.71215820312</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2175.44970703125</v>
+      </c>
+      <c r="F22">
+        <v>91.084063342318004</v>
+      </c>
+      <c r="G22">
+        <v>852.847412109375</v>
+      </c>
+      <c r="H22">
+        <v>80.934378468368394</v>
+      </c>
+      <c r="I22">
+        <v>2291.72509765625</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23">
-        <v>91.6666666666666</v>
+        <v>86.210154452842502</v>
       </c>
       <c r="C23">
-        <v>365.688385009765</v>
+        <v>1313.13891601562</v>
       </c>
       <c r="D23">
-        <v>79.8661209766925</v>
+        <v>82.422308546059895</v>
       </c>
       <c r="E23">
-        <v>2390.15991210937</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2079.06616210937</v>
+      </c>
+      <c r="F23">
+        <v>92.076076240551998</v>
+      </c>
+      <c r="G23">
+        <v>794.68450927734295</v>
+      </c>
+      <c r="H23">
+        <v>80.476553829078796</v>
+      </c>
+      <c r="I23">
+        <v>2327.4306640625</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24">
-        <v>92.112005856515296</v>
+        <v>86.401539448364304</v>
       </c>
       <c r="C24">
-        <v>365.0380859375</v>
+        <v>1336.701171875</v>
       </c>
       <c r="D24">
-        <v>80.826859045504904</v>
+        <v>82.158712541620403</v>
       </c>
       <c r="E24">
-        <v>2301.91918945312</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2091.509765625</v>
+      </c>
+      <c r="F24">
+        <v>91.861770365618995</v>
+      </c>
+      <c r="G24">
+        <v>820.796630859375</v>
+      </c>
+      <c r="H24">
+        <v>81.902053274139803</v>
+      </c>
+      <c r="I24">
+        <v>2123.58569335937</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25">
-        <v>91.938665710186498</v>
+        <v>87.034137175070398</v>
       </c>
       <c r="C25">
-        <v>375.25775146484301</v>
+        <v>1300.89575195312</v>
       </c>
       <c r="D25">
-        <v>81.586431742508296</v>
+        <v>80.774833518312903</v>
       </c>
       <c r="E25">
-        <v>2194.69458007812</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2254.86450195312</v>
+      </c>
+      <c r="F25">
+        <v>92.405261509552105</v>
+      </c>
+      <c r="G25">
+        <v>781.921875</v>
+      </c>
+      <c r="H25">
+        <v>80.795643729189706</v>
+      </c>
+      <c r="I25">
+        <v>2332.88623046875</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26">
-        <v>92.528129395218002</v>
+        <v>87.672123623011004</v>
       </c>
       <c r="C26">
-        <v>357.82943725585898</v>
+        <v>1262.611328125</v>
       </c>
       <c r="D26">
-        <v>80.982935627081005</v>
+        <v>82.592258601553795</v>
       </c>
       <c r="E26">
-        <v>2292.12841796875</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2017.42016601562</v>
+      </c>
+      <c r="F26">
+        <v>92.480110159118695</v>
+      </c>
+      <c r="G26">
+        <v>783.07574462890602</v>
+      </c>
+      <c r="H26">
+        <v>81.527469478357304</v>
+      </c>
+      <c r="I26">
+        <v>2239.87548828125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27">
-        <v>92.146551724137893</v>
+        <v>87.885133113969403</v>
       </c>
       <c r="C27">
-        <v>369.75750732421801</v>
+        <v>1286.38903808593</v>
       </c>
       <c r="D27">
-        <v>80.674250832408404</v>
+        <v>82.977247502774702</v>
       </c>
       <c r="E27">
-        <v>2288.2412109375</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2004.97253417968</v>
+      </c>
+      <c r="F27">
+        <v>92.850732874663393</v>
+      </c>
+      <c r="G27">
+        <v>770.153076171875</v>
+      </c>
+      <c r="H27">
+        <v>81.610710321864602</v>
+      </c>
+      <c r="I27">
+        <v>2245.26635742187</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28">
-        <v>92.642083897158301</v>
+        <v>88.052223522527797</v>
       </c>
       <c r="C28">
-        <v>361.91903686523398</v>
+        <v>1269.45593261718</v>
       </c>
       <c r="D28">
-        <v>81.725166481686998</v>
+        <v>83.199223085460503</v>
       </c>
       <c r="E28">
-        <v>2233.74194335937</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1905.11328125</v>
+      </c>
+      <c r="F28">
+        <v>93.099034523112906</v>
+      </c>
+      <c r="G28">
+        <v>755.082763671875</v>
+      </c>
+      <c r="H28">
+        <v>82.037319644839002</v>
+      </c>
+      <c r="I28">
+        <v>2217.97143554687</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29">
-        <v>92.936586985391699</v>
+        <v>88.280131691955305</v>
       </c>
       <c r="C29">
-        <v>345.54544067382801</v>
+        <v>1268.26306152343</v>
       </c>
       <c r="D29">
-        <v>82.196864594894507</v>
+        <v>81.634988901220794</v>
       </c>
       <c r="E29">
-        <v>2151.04418945312</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2140.55859375</v>
+      </c>
+      <c r="F29">
+        <v>93.3116232464929</v>
+      </c>
+      <c r="G29">
+        <v>751.94622802734295</v>
+      </c>
+      <c r="H29">
+        <v>81.749445061043204</v>
+      </c>
+      <c r="I29">
+        <v>2305.20751953125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30">
-        <v>92.853650586701406</v>
+        <v>88.873318385650194</v>
       </c>
       <c r="C30">
-        <v>364.434967041015</v>
+        <v>1246.509765625</v>
       </c>
       <c r="D30">
-        <v>81.159822419533796</v>
+        <v>82.151775804661398</v>
       </c>
       <c r="E30">
-        <v>2282.61254882812</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2078.16845703125</v>
+      </c>
+      <c r="F30">
+        <v>93.497757847533606</v>
+      </c>
+      <c r="G30">
+        <v>746.01080322265602</v>
+      </c>
+      <c r="H30">
+        <v>81.707824639289598</v>
+      </c>
+      <c r="I30">
+        <v>2293.68505859375</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="B31">
-        <v>93.1381957773512</v>
+        <v>89.335712325006796</v>
       </c>
       <c r="C31">
-        <v>342.32687377929602</v>
+        <v>1225.48474121093</v>
       </c>
       <c r="D31">
-        <v>80.573668146503806</v>
+        <v>83.820061043285193</v>
       </c>
       <c r="E31">
-        <v>2352.2705078125</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1905.72534179687</v>
+      </c>
+      <c r="F31">
+        <v>93.816909140817998</v>
+      </c>
+      <c r="G31">
+        <v>717.19439697265602</v>
+      </c>
+      <c r="H31">
+        <v>82.6165371809101</v>
+      </c>
+      <c r="I31">
+        <v>2216.39794921875</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
       <c r="B32">
-        <v>93.156819610307906</v>
+        <v>89.248251748251704</v>
       </c>
       <c r="C32">
-        <v>350.34808349609301</v>
+        <v>1244.13098144531</v>
       </c>
       <c r="D32">
-        <v>80.306603773584897</v>
+        <v>83.084766925638107</v>
       </c>
       <c r="E32">
-        <v>2466.52880859375</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1978.43786621093</v>
+      </c>
+      <c r="F32">
+        <v>93.884480903711605</v>
+      </c>
+      <c r="G32">
+        <v>715.03570556640602</v>
+      </c>
+      <c r="H32">
+        <v>82.977247502774702</v>
+      </c>
+      <c r="I32">
+        <v>2135.60034179687</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
       <c r="B33">
-        <v>93.638048177887498</v>
+        <v>89.289480622198795</v>
       </c>
       <c r="C33">
-        <v>336.04794311523398</v>
+        <v>1240.15295410156</v>
       </c>
       <c r="D33">
-        <v>79.658018867924497</v>
+        <v>82.682436182019899</v>
       </c>
       <c r="E33">
-        <v>2523.54565429687</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2013.41235351562</v>
+      </c>
+      <c r="F33">
+        <v>93.952675982072194</v>
+      </c>
+      <c r="G33">
+        <v>714.18878173828102</v>
+      </c>
+      <c r="H33">
+        <v>82.373751387347397</v>
+      </c>
+      <c r="I33">
+        <v>2218.849609375</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
       <c r="B34">
-        <v>93.154219793563996</v>
+        <v>90.001292657704198</v>
       </c>
       <c r="C34">
-        <v>366.02056884765602</v>
+        <v>1186.21240234375</v>
       </c>
       <c r="D34">
-        <v>81.083518312985504</v>
+        <v>83.764567147613704</v>
       </c>
       <c r="E34">
-        <v>2379.1025390625</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1897.64978027343</v>
+      </c>
+      <c r="F34">
+        <v>94.040847983453901</v>
+      </c>
+      <c r="G34">
+        <v>711.91174316406205</v>
+      </c>
+      <c r="H34">
+        <v>82.959905660377302</v>
+      </c>
+      <c r="I34">
+        <v>2144.63012695312</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
       <c r="B35">
-        <v>93.514925373134304</v>
+        <v>90.537027643925896</v>
       </c>
       <c r="C35">
-        <v>355.20574951171801</v>
+        <v>1171.10534667968</v>
       </c>
       <c r="D35">
-        <v>80.452275249722504</v>
+        <v>84.267480577136496</v>
       </c>
       <c r="E35">
-        <v>2477.80151367187</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1813.25109863281</v>
+      </c>
+      <c r="F35">
+        <v>94.4521937610956</v>
+      </c>
+      <c r="G35">
+        <v>672.05303955078102</v>
+      </c>
+      <c r="H35">
+        <v>83.216564927857902</v>
+      </c>
+      <c r="I35">
+        <v>2113.85815429687</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
       <c r="B36">
-        <v>93.650910158543695</v>
+        <v>90.4927824788452</v>
       </c>
       <c r="C36">
-        <v>342.49667358398398</v>
+        <v>1170.17785644531</v>
       </c>
       <c r="D36">
-        <v>81.170227524972205</v>
+        <v>83.833934517203105</v>
       </c>
       <c r="E36">
-        <v>2334.94311523437</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1879.61987304687</v>
+      </c>
+      <c r="F36">
+        <v>94.577526132404103</v>
+      </c>
+      <c r="G36">
+        <v>677.02142333984295</v>
+      </c>
+      <c r="H36">
+        <v>83.157602663706996</v>
+      </c>
+      <c r="I36">
+        <v>2204.31298828125</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
       <c r="B37">
-        <v>94.129116117850899</v>
+        <v>90.877718055216206</v>
       </c>
       <c r="C37">
-        <v>338.94680786132801</v>
+        <v>1155.0625</v>
       </c>
       <c r="D37">
-        <v>81.409544950055405</v>
+        <v>83.525249722530504</v>
       </c>
       <c r="E37">
-        <v>2334.84643554687</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1940.25573730468</v>
+      </c>
+      <c r="F37">
+        <v>94.612753481553796</v>
+      </c>
+      <c r="G37">
+        <v>664.48504638671795</v>
+      </c>
+      <c r="H37">
+        <v>83.480160932297395</v>
+      </c>
+      <c r="I37">
+        <v>2164.56689453125</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38">
-        <v>94.073337123365505</v>
+        <v>91.404750479846399</v>
       </c>
       <c r="C38">
-        <v>349.64431762695301</v>
+        <v>1106.51745605468</v>
       </c>
       <c r="D38">
-        <v>81.891648168701394</v>
+        <v>84.978496115427305</v>
       </c>
       <c r="E38">
-        <v>2239.37817382812</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1771.0947265625</v>
+      </c>
+      <c r="F38">
+        <v>94.964611324376193</v>
+      </c>
+      <c r="G38">
+        <v>644.64056396484295</v>
+      </c>
+      <c r="H38">
+        <v>82.1552441731409</v>
+      </c>
+      <c r="I38">
+        <v>2353.33618164062</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="B39">
-        <v>94.050615212527902</v>
+        <v>91.515437190666901</v>
       </c>
       <c r="C39">
-        <v>351.19265747070301</v>
+        <v>1104.1455078125</v>
       </c>
       <c r="D39">
-        <v>80.663845726969996</v>
+        <v>83.743756936736901</v>
       </c>
       <c r="E39">
-        <v>2431.49682617187</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1905.68225097656</v>
+      </c>
+      <c r="F39">
+        <v>95.268677822295501</v>
+      </c>
+      <c r="G39">
+        <v>629.73883056640602</v>
+      </c>
+      <c r="H39">
+        <v>83.809655937846799</v>
+      </c>
+      <c r="I39">
+        <v>2162.04711914062</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
       <c r="B40">
-        <v>93.928964757709196</v>
+        <v>91.500694766095407</v>
       </c>
       <c r="C40">
-        <v>349.62228393554602</v>
+        <v>1120.23229980468</v>
       </c>
       <c r="D40">
-        <v>81.319367369589301</v>
+        <v>83.039678135405097</v>
       </c>
       <c r="E40">
-        <v>2337.61962890625</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1982.71911621093</v>
+      </c>
+      <c r="F40">
+        <v>95.093214451134699</v>
+      </c>
+      <c r="G40">
+        <v>653.90740966796795</v>
+      </c>
+      <c r="H40">
+        <v>83.240843507214194</v>
+      </c>
+      <c r="I40">
+        <v>2204.69799804687</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
       <c r="B41">
-        <v>94.116052060737502</v>
+        <v>91.728317778283596</v>
       </c>
       <c r="C41">
-        <v>354.74203491210898</v>
+        <v>1117.91198730468</v>
       </c>
       <c r="D41">
-        <v>82.630410654827898</v>
+        <v>85.092952275249701</v>
       </c>
       <c r="E41">
-        <v>2258.861328125</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1796.28869628906</v>
+      </c>
+      <c r="F41">
+        <v>95.398930116093695</v>
+      </c>
+      <c r="G41">
+        <v>626.82470703125</v>
+      </c>
+      <c r="H41">
+        <v>82.491675915649196</v>
+      </c>
+      <c r="I41">
+        <v>2293.16943359375</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
       <c r="B42">
-        <v>92.267189758414204</v>
+        <v>91.993061772605103</v>
       </c>
       <c r="C42">
-        <v>1178.91967773437</v>
+        <v>1110.51672363281</v>
       </c>
       <c r="D42">
-        <v>81.506659267480501</v>
+        <v>84.721836847946705</v>
       </c>
       <c r="E42">
-        <v>2292.0498046875</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1827.52429199218</v>
+      </c>
+      <c r="F42">
+        <v>95.551700984780595</v>
+      </c>
+      <c r="G42">
+        <v>614.77990722656205</v>
+      </c>
+      <c r="H42">
+        <v>82.561043285238597</v>
+      </c>
+      <c r="I42">
+        <v>2363.4287109375</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
       <c r="B43">
-        <v>92.863345521023703</v>
+        <v>92.083975346687197</v>
       </c>
       <c r="C43">
-        <v>1242.81567382812</v>
+        <v>1086.02966308593</v>
       </c>
       <c r="D43">
-        <v>82.571448390677006</v>
+        <v>84.995837957824605</v>
       </c>
       <c r="E43">
-        <v>2180.37182617187</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1824.94543457031</v>
+      </c>
+      <c r="F43">
+        <v>95.578362315650395</v>
+      </c>
+      <c r="G43">
+        <v>620.25762939453102</v>
+      </c>
+      <c r="H43">
+        <v>83.396920088790196</v>
+      </c>
+      <c r="I43">
+        <v>2288.3818359375</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
       <c r="B44">
-        <v>92.950167504187604</v>
+        <v>92.393893460372396</v>
       </c>
       <c r="C44">
-        <v>1300.27978515625</v>
+        <v>1073.27416992187</v>
       </c>
       <c r="D44">
-        <v>83.109045504994398</v>
+        <v>84.610849056603698</v>
       </c>
       <c r="E44">
-        <v>2101.32934570312</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1827.40759277343</v>
+      </c>
+      <c r="F44">
+        <v>95.839649198787299</v>
+      </c>
+      <c r="G44">
+        <v>587.20587158203102</v>
+      </c>
+      <c r="H44">
+        <v>83.2824639289678</v>
+      </c>
+      <c r="I44">
+        <v>2253.14233398437</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
       <c r="B45">
-        <v>93.052118775131405</v>
+        <v>92.275729810355799</v>
       </c>
       <c r="C45">
-        <v>1369.96936035156</v>
+        <v>1085.75952148437</v>
       </c>
       <c r="D45">
-        <v>82.450055493895604</v>
+        <v>84.621254162042106</v>
       </c>
       <c r="E45">
-        <v>2157.23950195312</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1886.86938476562</v>
+      </c>
+      <c r="F45">
+        <v>95.759642020029801</v>
+      </c>
+      <c r="G45">
+        <v>606.40142822265602</v>
+      </c>
+      <c r="H45">
+        <v>83.220033296337405</v>
+      </c>
+      <c r="I45">
+        <v>2256.29711914062</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
       <c r="B46">
-        <v>93.361716123373697</v>
+        <v>92.745910234899299</v>
       </c>
       <c r="C46">
-        <v>1382.3056640625</v>
+        <v>1053.72888183593</v>
       </c>
       <c r="D46">
-        <v>83.719478357380595</v>
+        <v>85.242092119866797</v>
       </c>
       <c r="E46">
-        <v>2072.63012695312</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1792.50744628906</v>
+      </c>
+      <c r="F46">
+        <v>95.949559563758299</v>
+      </c>
+      <c r="G46">
+        <v>589.73431396484295</v>
+      </c>
+      <c r="H46">
+        <v>83.376109877913393</v>
+      </c>
+      <c r="I46">
+        <v>2288.77709960937</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
       <c r="B47">
-        <v>93.640867516629697</v>
+        <v>92.631117076192396</v>
       </c>
       <c r="C47">
-        <v>1365.76428222656</v>
+        <v>1065.38354492187</v>
       </c>
       <c r="D47">
-        <v>84.270948945615899</v>
+        <v>84.985432852386197</v>
       </c>
       <c r="E47">
-        <v>2024.6484375</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1849.029296875</v>
+      </c>
+      <c r="F47">
+        <v>96.012285773280993</v>
+      </c>
+      <c r="G47">
+        <v>584.05822753906205</v>
+      </c>
+      <c r="H47">
+        <v>83.820061043285193</v>
+      </c>
+      <c r="I47">
+        <v>2209.47607421875</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
       <c r="B48">
-        <v>94.075220656040003</v>
+        <v>92.961906701975906</v>
       </c>
       <c r="C48">
-        <v>1352.654296875</v>
+        <v>1045.51782226562</v>
       </c>
       <c r="D48">
-        <v>83.660516093229703</v>
+        <v>85.464067702552697</v>
       </c>
       <c r="E48">
-        <v>2116.25537109375</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1786.01525878906</v>
+      </c>
+      <c r="F48">
+        <v>96.223772662456696</v>
+      </c>
+      <c r="G48">
+        <v>573.69512939453102</v>
+      </c>
+      <c r="H48">
+        <v>83.188817980022193</v>
+      </c>
+      <c r="I48">
+        <v>2347.05859375</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
       <c r="B49">
-        <v>94.195643986944503</v>
+        <v>93.229585679806902</v>
       </c>
       <c r="C49">
-        <v>1383.27502441406</v>
+        <v>1012.60174560546</v>
       </c>
       <c r="D49">
-        <v>83.684794672585994</v>
+        <v>85.200471698113205</v>
       </c>
       <c r="E49">
-        <v>2113.1572265625</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1798.9091796875</v>
+      </c>
+      <c r="F49">
+        <v>96.108205953338697</v>
+      </c>
+      <c r="G49">
+        <v>574.67864990234295</v>
+      </c>
+      <c r="H49">
+        <v>83.792314095449498</v>
+      </c>
+      <c r="I49">
+        <v>2233.3525390625</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
       <c r="B50">
-        <v>94.601966191104097</v>
+        <v>93.129221295192593</v>
       </c>
       <c r="C50">
-        <v>1338.25512695312</v>
+        <v>1024.84387207031</v>
       </c>
       <c r="D50">
-        <v>83.854744728079893</v>
+        <v>85.658296337402803</v>
       </c>
       <c r="E50">
-        <v>2127.11254882812</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1762.57202148437</v>
+      </c>
+      <c r="F50">
+        <v>96.208283671036895</v>
+      </c>
+      <c r="G50">
+        <v>572.38702392578102</v>
+      </c>
+      <c r="H50">
+        <v>83.4350721420643</v>
+      </c>
+      <c r="I50">
+        <v>2343.8125</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
       <c r="B51">
-        <v>94.895881138136701</v>
+        <v>93.309790072591696</v>
       </c>
       <c r="C51">
-        <v>1315.97595214843</v>
+        <v>1012.53485107421</v>
       </c>
       <c r="D51">
-        <v>83.605022197558199</v>
+        <v>85.491814650388406</v>
       </c>
       <c r="E51">
-        <v>2225.474609375</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1774.80822753906</v>
+      </c>
+      <c r="F51">
+        <v>96.363056700019598</v>
+      </c>
+      <c r="G51">
+        <v>559.172119140625</v>
+      </c>
+      <c r="H51">
+        <v>82.921753607103199</v>
+      </c>
+      <c r="I51">
+        <v>2359.9111328125</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
       </c>
       <c r="B52">
-        <v>95.246672533274605</v>
+        <v>93.470149253731293</v>
       </c>
       <c r="C52">
-        <v>1304.38024902343</v>
+        <v>1009.50109863281</v>
       </c>
       <c r="D52">
-        <v>83.9483906770255</v>
+        <v>85.932297447280803</v>
       </c>
       <c r="E52">
-        <v>2207.3984375</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1771.03063964843</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>51</v>
       </c>
       <c r="B53">
-        <v>95.544580604267907</v>
+        <v>93.8625047874377</v>
       </c>
       <c r="C53">
-        <v>1270.52404785156</v>
+        <v>992.16046142578102</v>
       </c>
       <c r="D53">
-        <v>84.048973362929999</v>
+        <v>85.873335183129797</v>
       </c>
       <c r="E53">
-        <v>2180.703125</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1759.43676757812</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
       <c r="B54">
-        <v>95.631290027447307</v>
+        <v>93.723978046934107</v>
       </c>
       <c r="C54">
-        <v>1259.90454101562</v>
+        <v>977.92901611328102</v>
       </c>
       <c r="D54">
-        <v>84.080188679245197</v>
+        <v>86.147336293007697</v>
       </c>
       <c r="E54">
-        <v>2233.845703125</v>
+        <v>1755.59545898437</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>94.120534879371604</v>
+      </c>
+      <c r="C55">
+        <v>969.07257080078102</v>
+      </c>
+      <c r="D55">
+        <v>86.140399556048806</v>
+      </c>
+      <c r="E55">
+        <v>1730.048828125</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>94.016916250693299</v>
+      </c>
+      <c r="C56">
+        <v>961.09857177734295</v>
+      </c>
+      <c r="D56">
+        <v>85.519561598224101</v>
+      </c>
+      <c r="E56">
+        <v>1880.046875</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <v>94.335009140767795</v>
+      </c>
+      <c r="C57">
+        <v>937.07672119140602</v>
+      </c>
+      <c r="D57">
+        <v>85.772752497225298</v>
+      </c>
+      <c r="E57">
+        <v>1809.19494628906</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58">
+        <v>94.202898550724598</v>
+      </c>
+      <c r="C58">
+        <v>951.370361328125</v>
+      </c>
+      <c r="D58">
+        <v>86.230577136514896</v>
+      </c>
+      <c r="E58">
+        <v>1723.50231933593</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>94.340215439856294</v>
+      </c>
+      <c r="C59">
+        <v>924.67712402343705</v>
+      </c>
+      <c r="D59">
+        <v>85.2455604883462</v>
+      </c>
+      <c r="E59">
+        <v>1869.41357421875</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="B60">
+        <v>94.570729537366503</v>
+      </c>
+      <c r="C60">
+        <v>898.95684814453102</v>
+      </c>
+      <c r="D60">
+        <v>86.331159822419494</v>
+      </c>
+      <c r="E60">
+        <v>1769.6025390625</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <v>94.750881834215093</v>
+      </c>
+      <c r="C61">
+        <v>885.01812744140602</v>
+      </c>
+      <c r="D61">
+        <v>85.828246392896702</v>
+      </c>
+      <c r="E61">
+        <v>1853.14965820312</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>60</v>
+      </c>
+      <c r="B62">
+        <v>94.694055944055904</v>
+      </c>
+      <c r="C62">
+        <v>891.15576171875</v>
+      </c>
+      <c r="D62">
+        <v>85.762347391786903</v>
+      </c>
+      <c r="E62">
+        <v>1813.45959472656</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>61</v>
+      </c>
+      <c r="B63">
+        <v>94.794194107452299</v>
+      </c>
+      <c r="C63">
+        <v>890.88690185546795</v>
+      </c>
+      <c r="D63">
+        <v>86.043285238623696</v>
+      </c>
+      <c r="E63">
+        <v>1853.36926269531</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>62</v>
+      </c>
+      <c r="B64">
+        <v>94.7487113402061</v>
+      </c>
+      <c r="C64">
+        <v>907.13995361328102</v>
+      </c>
+      <c r="D64">
+        <v>86.3380965593784</v>
+      </c>
+      <c r="E64">
+        <v>1824.70068359375</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>63</v>
+      </c>
+      <c r="B65">
+        <v>94.925468483816005</v>
+      </c>
+      <c r="C65">
+        <v>880.83465576171795</v>
+      </c>
+      <c r="D65">
+        <v>85.644422863485005</v>
+      </c>
+      <c r="E65">
+        <v>1885.46044921875</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>64</v>
+      </c>
+      <c r="B66">
+        <v>95.086570945945894</v>
+      </c>
+      <c r="C66">
+        <v>865.154296875</v>
+      </c>
+      <c r="D66">
+        <v>86.095310765815697</v>
+      </c>
+      <c r="E66">
+        <v>1910.61962890625</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>64</v>
+      </c>
+      <c r="B67">
+        <v>97.548742011164094</v>
+      </c>
+      <c r="C67">
+        <v>887.9287109375</v>
+      </c>
+      <c r="D67">
+        <v>83.990011098779107</v>
+      </c>
+      <c r="E67">
+        <v>2608.65478515625</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>65</v>
+      </c>
+      <c r="B68">
+        <v>97.633686594935597</v>
+      </c>
+      <c r="C68">
+        <v>874.735595703125</v>
+      </c>
+      <c r="D68">
+        <v>84.898723640399496</v>
+      </c>
+      <c r="E68">
+        <v>2469.38842773437</v>
       </c>
     </row>
   </sheetData>

</xml_diff>